<commit_message>
Change method for create file for print. Set path to Original.xlsx in .jar. Package mavenproject1... to a running program
</commit_message>
<xml_diff>
--- a/target/classes/by/bobruisk/zhelnov/myproject/mavenproject1/Original.xlsx
+++ b/target/classes/by/bobruisk/zhelnov/myproject/mavenproject1/Original.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="286">
   <si>
     <t>Эритроциты</t>
   </si>
@@ -1136,10 +1136,25 @@
     <t>2000</t>
   </si>
   <si>
-    <t>OOO</t>
+    <t>Лынькова</t>
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>Желнов</t>
+  </si>
+  <si>
+    <t>Антон</t>
+  </si>
+  <si>
+    <t>Олегович</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>103</t>
   </si>
 </sst>
 </file>
@@ -1381,7 +1396,7 @@
       <bottom style="thin"/>
     </border>
   </borders>
-  <cellStyleXfs count="104">
+  <cellStyleXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment/>
       <protection/>
@@ -1405,6 +1420,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2213,7 +2242,7 @@
     <row r="6" spans="1:13" ht="12.75" customHeight="1">
       <c r="A6" s="25" t="str">
         <f>CONCATENATE("1. Ф.И.О: "," ",C55," ",E55," ",F55," ")</f>
-        <v>1. Ф.И.О:  OOO OOO OOO </v>
+        <v>1. Ф.И.О:  Желнов Антон Олегович </v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
@@ -2223,7 +2252,7 @@
       <c r="G6" s="25"/>
       <c r="H6" s="25" t="str">
         <f>CONCATENATE("1. Ф.И.О: "," ",C55," ",E55," ",F55," ")</f>
-        <v>1. Ф.И.О:  OOO OOO OOO </v>
+        <v>1. Ф.И.О:  Желнов Антон Олегович </v>
       </c>
       <c r="I6" s="25"/>
       <c r="J6" s="25"/>
@@ -2274,7 +2303,7 @@
     <row r="9" spans="1:13" ht="12.75" customHeight="1">
       <c r="A9" s="25" t="str">
         <f>IF(VALUE(G57)=0,CONCATENATE("4. Адрес: ",C57,", дом ",E57),IF(F57="",CONCATENATE("4. Адрес: ",C57,", дом ",E57,F57,", квартира ",G57),CONCATENATE("4. Адрес:  ",C57,", дом ",E57,", корпус ",F57,", квартира ",G57)))</f>
-        <v>4. Адрес: OOO, дом 1, квартира 1</v>
+        <v>4. Адрес: Лынькова, дом 75, квартира 103</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="25"/>
@@ -2284,7 +2313,7 @@
       <c r="G9" s="25"/>
       <c r="H9" s="25" t="str">
         <f>IF(VALUE(G57)=0,CONCATENATE("4. Адрес: ",C57,", дом ",E57),IF(F57="",CONCATENATE("4. Адрес: ",C57,", дом ",E57,F57,", квартира ",G57),CONCATENATE("4. Адрес:  ",C57,", дом ",E57,", корпус ",F57,", квартира ",G57)))</f>
-        <v>4. Адрес: OOO, дом 1, квартира 1</v>
+        <v>4. Адрес: Лынькова, дом 75, квартира 103</v>
       </c>
       <c r="I9" s="25"/>
       <c r="J9" s="25"/>
@@ -2954,7 +2983,7 @@
     <row r="39" spans="1:7" ht="15">
       <c r="A39" s="2" t="str">
         <f>CONCATENATE("1. Ф.И.О: "," ",C55," ",E55," ",F55," ")</f>
-        <v>1. Ф.И.О:  OOO OOO OOO </v>
+        <v>1. Ф.И.О:  Желнов Антон Олегович </v>
       </c>
       <c r="G39" s="17"/>
     </row>
@@ -2972,7 +3001,7 @@
     <row r="42" ht="15">
       <c r="A42" s="25" t="str">
         <f>IF(VALUE(G57)=0,CONCATENATE("проспект/улица/ переулок/проезд ",C57,", дом ",E57),IF(F57="",CONCATENATE("проспект/улица/ переулок/проезд ",C57," дом ",E57,F57," квартира ",G57),CONCATENATE("Адрес: улица ",C57," дом ",E57," корпус ",F57," квартира ",G57)))</f>
-        <v>проспект/улица/ переулок/проезд OOO дом 1 квартира 1</v>
+        <v>проспект/улица/ переулок/проезд Лынькова дом 75 квартира 103</v>
       </c>
     </row>
     <row r="43" ht="15">
@@ -3103,14 +3132,14 @@
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="37" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D55" s="38"/>
       <c r="E55" s="29" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="F55" s="37" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="G55" s="53"/>
       <c r="H55" s="53"/>
@@ -3152,13 +3181,13 @@
       </c>
       <c r="D57" s="38"/>
       <c r="E57" s="28" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="F57" s="29" t="s">
         <v>272</v>
       </c>
       <c r="G57" s="37" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="H57" s="53"/>
       <c r="I57" s="38"/>
@@ -3348,11 +3377,11 @@
     <row r="6" spans="1:8" ht="11.85" customHeight="1">
       <c r="A6" s="2" t="str">
         <f>CONCATENATE("1. Ф.И.О. пациента: ",Лист1!C55," ",Лист1!E55," ",Лист1!F55," ")</f>
-        <v>1. Ф.И.О. пациента: OOO OOO OOO </v>
+        <v>1. Ф.И.О. пациента: Желнов Антон Олегович </v>
       </c>
       <c r="H6" s="2" t="str">
         <f>CONCATENATE("1. Ф.И.О. пациента: ",Лист1!C55," ",Лист1!E55," ",Лист1!F55," ")</f>
-        <v>1. Ф.И.О. пациента: OOO OOO OOO </v>
+        <v>1. Ф.И.О. пациента: Желнов Антон Олегович </v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="11.85" customHeight="1">
@@ -3369,11 +3398,11 @@
     <row r="8" spans="1:8" ht="11.85" customHeight="1">
       <c r="A8" s="2" t="str">
         <f>IF(VALUE(Лист1!G57)=0,CONCATENATE("4. Адрес: ",Лист1!C57,", дом ",Лист1!E57),IF(Лист1!F57="",CONCATENATE("4. Адрес: ",Лист1!C57,", дом ",Лист1!E57,Лист1!F57,", квартира ",Лист1!G57),CONCATENATE("4. Адрес:  ",Лист1!C57,", дом ",Лист1!E57,", корпус ",Лист1!F57,", квартира ",Лист1!G57)))</f>
-        <v>4. Адрес: OOO, дом 1, квартира 1</v>
+        <v>4. Адрес: Лынькова, дом 75, квартира 103</v>
       </c>
       <c r="H8" s="2" t="str">
         <f>IF(VALUE(Лист1!G57)=0,CONCATENATE("4. Адрес: ",Лист1!C57,", дом ",Лист1!E57),IF(Лист1!F57="",CONCATENATE("4. Адрес: ",Лист1!C57,", дом ",Лист1!E57,Лист1!F57,", квартира ",Лист1!G57),CONCATENATE("4. Адрес:  ",Лист1!C57,", дом ",Лист1!E57,", корпус ",Лист1!F57,", квартира ",Лист1!G57)))</f>
-        <v>4. Адрес: OOO, дом 1, квартира 1</v>
+        <v>4. Адрес: Лынькова, дом 75, квартира 103</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="11.85" customHeight="1">
@@ -4443,18 +4472,18 @@
       </c>
       <c r="I7" s="18" t="str">
         <f>CONCATENATE("1. Фамилия :  ",Лист1!C55,"                                                            2. Имя:  ",Лист1!E55)</f>
-        <v>1. Фамилия :  OOO                                                            2. Имя:  OOO</v>
+        <v>1. Фамилия :  Желнов                                                            2. Имя:  Антон</v>
       </c>
       <c r="M7" s="20"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1">
       <c r="A8" s="21" t="str">
         <f>CONCATENATE("1. Ф.И.О. пациента: ",Лист1!C55," ",Лист1!E55," ",Лист1!F55," ")</f>
-        <v>1. Ф.И.О. пациента: OOO OOO OOO </v>
+        <v>1. Ф.И.О. пациента: Желнов Антон Олегович </v>
       </c>
       <c r="I8" s="18" t="str">
         <f>CONCATENATE("3. Отчество:  ",Лист1!F55,"")</f>
-        <v>3. Отчество:  OOO</v>
+        <v>3. Отчество:  Олегович</v>
       </c>
       <c r="L8" s="18" t="str">
         <f>CONCATENATE("4. Число, месяц, год рождения: ",Лист1!D56,".",Лист1!E56,".",Лист1!F56)</f>
@@ -4475,7 +4504,7 @@
     <row r="10" spans="1:13" ht="15.75" customHeight="1">
       <c r="A10" s="21" t="str">
         <f>IF(VALUE(Лист1!G57)=0,CONCATENATE("4. Адрес: ",Лист1!C57,", дом ",Лист1!E57),IF(Лист1!F57="",CONCATENATE("4. Адрес: ",Лист1!C57,", дом ",Лист1!E57,Лист1!F57,", квартира ",Лист1!G57),CONCATENATE("4. Адрес:  ",Лист1!C57,", дом ",Лист1!E57,", корпус ",Лист1!F57,", квартира ",Лист1!G57)))</f>
-        <v>4. Адрес: OOO, дом 1, квартира 1</v>
+        <v>4. Адрес: Лынькова, дом 75, квартира 103</v>
       </c>
       <c r="I10" s="18" t="s">
         <v>143</v>
@@ -4489,7 +4518,7 @@
       </c>
       <c r="I11" s="18" t="str">
         <f>IF(Лист1!F57="",CONCATENATE("проспект/улица/переулок/проезд ",Лист1!C57,", дом ",Лист1!E57,Лист1!F57,", квартира ",Лист1!G57),CONCATENATE("проспект/улица/переулок/проезд ",Лист1!C57,", дом ",Лист1!E57,", корпус ",Лист1!F57,", квартира ",Лист1!G57))</f>
-        <v>проспект/улица/переулок/проезд OOO, дом 1, квартира 1</v>
+        <v>проспект/улица/переулок/проезд Лынькова, дом 75, квартира 103</v>
       </c>
       <c r="M11" s="20"/>
     </row>

</xml_diff>